<commit_message>
Add test case login_07. Clean all comments in util.js and commands.js.
</commit_message>
<xml_diff>
--- a/cypress/fixtures/testCaseCriteria/testCaseCriteria_contact.xlsx
+++ b/cypress/fixtures/testCaseCriteria/testCaseCriteria_contact.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\awika-portfolio\automationexercise\cypress\fixtures\testCaseCriteria\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0D609B5-2D6A-48E2-89CF-1820B4B166D1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{021F5CE8-F70F-4F53-85B4-372F58EC628E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="553" activeTab="1" xr2:uid="{63A55816-40FB-44DD-8B96-272E0273596B}"/>
   </bookViews>
@@ -623,8 +623,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5E12B883-930C-47C5-B78F-1CE0B70C744F}">
   <dimension ref="A1:Y2"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -711,8 +711,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8911E0E7-99F5-492F-AA20-746F86B5DC7B}">
   <dimension ref="A1:Y2"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -791,8 +791,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DA0E15DF-455A-49EC-BCB3-C2DAA22AE95D}">
   <dimension ref="A1:Y2"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -882,8 +882,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9F9BF6F9-A417-4D30-9082-65C0E356320E}">
   <dimension ref="A1:Y2"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -968,8 +968,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A968B7B4-F049-47F7-96D4-976DE1493C75}">
   <dimension ref="A1:Y2"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E24" sqref="E24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>